<commit_message>
first iteration of list component done. Sorting now works
</commit_message>
<xml_diff>
--- a/data/LOGBOG-CLIMBING-DATA.xlsx
+++ b/data/LOGBOG-CLIMBING-DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mw/Documents/projects/send-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F31A33-29BA-BF4F-94EE-5630360D1C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082C9D2D-2FE4-F44C-B4CA-ADEF0E87282F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7860,7 +7860,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1419266-817B-49F7-AE72-10008B17EA6B}" name="Tabel6" displayName="Tabel6" ref="A1:M186" totalsRowShown="0">
-  <autoFilter ref="A1:M186" xr:uid="{D1419266-817B-49F7-AE72-10008B17EA6B}"/>
+  <autoFilter ref="A1:M186" xr:uid="{D1419266-817B-49F7-AE72-10008B17EA6B}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Joachim"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M186">
     <sortCondition ref="B1:B186"/>
   </sortState>
@@ -8087,7 +8093,7 @@
   <dimension ref="A1:AC1007"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8196,7 +8202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -8231,7 +8237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -8266,7 +8272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -8301,7 +8307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -8336,7 +8342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>2021</v>
       </c>
@@ -8371,7 +8377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2021</v>
       </c>
@@ -8406,7 +8412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2021</v>
       </c>
@@ -8441,7 +8447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -8476,7 +8482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -8511,7 +8517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2021</v>
       </c>
@@ -8546,7 +8552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -8581,7 +8587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:29" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2021</v>
       </c>
@@ -8616,7 +8622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -8721,7 +8727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2021</v>
       </c>
@@ -8791,7 +8797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2021</v>
       </c>
@@ -8842,7 +8848,7 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
     </row>
-    <row r="21" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2021</v>
       </c>
@@ -8893,7 +8899,7 @@
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
     </row>
-    <row r="22" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>2021</v>
       </c>
@@ -8928,7 +8934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>2021</v>
       </c>
@@ -8963,7 +8969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>2021</v>
       </c>
@@ -8998,7 +9004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>2021</v>
       </c>
@@ -9068,7 +9074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>2021</v>
       </c>
@@ -9103,7 +9109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>2021</v>
       </c>
@@ -9138,7 +9144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:29" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>2021</v>
       </c>
@@ -9173,7 +9179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:29" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>2021</v>
       </c>
@@ -9208,7 +9214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:29" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>2020</v>
       </c>
@@ -9278,7 +9284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:27" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -9313,7 +9319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:27" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>2021</v>
       </c>
@@ -9348,7 +9354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:27" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>2021</v>
       </c>
@@ -9383,7 +9389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:27" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>2021</v>
       </c>
@@ -9418,7 +9424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:27" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>2021</v>
       </c>
@@ -9453,7 +9459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:27" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>2021</v>
       </c>
@@ -9488,7 +9494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:27" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>2021</v>
       </c>
@@ -9529,7 +9535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>2021</v>
       </c>
@@ -9564,7 +9570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:27" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>2021</v>
       </c>
@@ -9599,7 +9605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:27" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>2021</v>
       </c>
@@ -9634,7 +9640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:27" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>2021</v>
       </c>
@@ -9675,7 +9681,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>2021</v>
       </c>
@@ -9757,7 +9763,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:27" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>2021</v>
       </c>
@@ -9792,7 +9798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:27" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>2021</v>
       </c>
@@ -9827,7 +9833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -9888,7 +9894,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>2021</v>
       </c>
@@ -9949,7 +9955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>2021</v>
       </c>
@@ -9986,7 +9992,7 @@
       <c r="R50" s="6"/>
       <c r="S50" s="6"/>
     </row>
-    <row r="51" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>2021</v>
       </c>
@@ -10027,7 +10033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>2022</v>
       </c>
@@ -10068,7 +10074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>2022</v>
       </c>
@@ -10109,7 +10115,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>2022</v>
       </c>
@@ -10144,7 +10150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>2022</v>
       </c>
@@ -10179,7 +10185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>2022</v>
       </c>
@@ -10214,7 +10220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>2022</v>
       </c>
@@ -10249,7 +10255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>2022</v>
       </c>
@@ -10284,7 +10290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>2022</v>
       </c>
@@ -10319,7 +10325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>2022</v>
       </c>
@@ -10354,7 +10360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>2022</v>
       </c>
@@ -10389,7 +10395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>2022</v>
       </c>
@@ -10424,7 +10430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>2022</v>
       </c>
@@ -10459,7 +10465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>2022</v>
       </c>
@@ -10494,7 +10500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>2022</v>
       </c>
@@ -10529,7 +10535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>2022</v>
       </c>
@@ -10564,7 +10570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>2022</v>
       </c>
@@ -10599,7 +10605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>2022</v>
       </c>
@@ -10634,7 +10640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>2022</v>
       </c>
@@ -10669,7 +10675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>2022</v>
       </c>
@@ -10704,7 +10710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>2022</v>
       </c>
@@ -10739,7 +10745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>2022</v>
       </c>
@@ -10774,7 +10780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>2022</v>
       </c>
@@ -10809,7 +10815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>2021</v>
       </c>
@@ -10844,7 +10850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>2021</v>
       </c>
@@ -10879,7 +10885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>2021</v>
       </c>
@@ -10914,7 +10920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>2021</v>
       </c>
@@ -10949,7 +10955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>2021</v>
       </c>
@@ -10984,7 +10990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>2021</v>
       </c>
@@ -11019,7 +11025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>2021</v>
       </c>
@@ -11054,7 +11060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>2021</v>
       </c>
@@ -11089,7 +11095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>2021</v>
       </c>
@@ -11130,7 +11136,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>2021</v>
       </c>
@@ -11165,7 +11171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>2021</v>
       </c>
@@ -11200,7 +11206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>2021</v>
       </c>
@@ -11235,7 +11241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>2021</v>
       </c>
@@ -11270,7 +11276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>2021</v>
       </c>
@@ -11305,7 +11311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>2021</v>
       </c>
@@ -11340,7 +11346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>2021</v>
       </c>
@@ -11381,7 +11387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90">
         <v>2021</v>
       </c>
@@ -11416,7 +11422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>2021</v>
       </c>
@@ -11457,7 +11463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:13" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92">
         <v>2021</v>
       </c>
@@ -11751,7 +11757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100">
         <v>2021</v>
       </c>
@@ -11853,7 +11859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103">
         <v>2021</v>
       </c>
@@ -11888,7 +11894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104">
         <v>2021</v>
       </c>
@@ -11923,7 +11929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105">
         <v>2021</v>
       </c>
@@ -11958,7 +11964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106">
         <v>2021</v>
       </c>
@@ -12133,7 +12139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111">
         <v>2021</v>
       </c>
@@ -12174,7 +12180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112">
         <v>2021</v>
       </c>
@@ -12209,7 +12215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113">
         <v>2021</v>
       </c>
@@ -12244,7 +12250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114">
         <v>2021</v>
       </c>
@@ -12279,7 +12285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -12314,7 +12320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116">
         <v>2021</v>
       </c>
@@ -12384,7 +12390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118">
         <v>2021</v>
       </c>
@@ -12419,7 +12425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A119">
         <v>2021</v>
       </c>
@@ -12454,7 +12460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120">
         <v>2021</v>
       </c>
@@ -12489,7 +12495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A121">
         <v>2021</v>
       </c>
@@ -12524,7 +12530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122">
         <v>2021</v>
       </c>
@@ -12559,7 +12565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123">
         <v>2021</v>
       </c>
@@ -12594,7 +12600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A124">
         <v>2021</v>
       </c>
@@ -12664,7 +12670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126">
         <v>2021</v>
       </c>
@@ -12699,7 +12705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A127">
         <v>2021</v>
       </c>
@@ -12804,7 +12810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130">
         <v>2020</v>
       </c>
@@ -12839,7 +12845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131">
         <v>2021</v>
       </c>
@@ -12874,7 +12880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132">
         <v>2021</v>
       </c>
@@ -12909,7 +12915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133">
         <v>2021</v>
       </c>
@@ -12944,7 +12950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134">
         <v>2021</v>
       </c>
@@ -12979,7 +12985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A135">
         <v>2021</v>
       </c>
@@ -13014,7 +13020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136">
         <v>2021</v>
       </c>
@@ -13049,7 +13055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A137">
         <v>2021</v>
       </c>
@@ -13084,7 +13090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:13" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A138">
         <v>2021</v>
       </c>
@@ -13154,7 +13160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A140">
         <v>2021</v>
       </c>
@@ -13189,7 +13195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A141">
         <v>2021</v>
       </c>
@@ -13224,7 +13230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A142">
         <v>2021</v>
       </c>
@@ -13259,7 +13265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A143">
         <v>2021</v>
       </c>
@@ -13294,7 +13300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A144">
         <v>2021</v>
       </c>
@@ -13329,7 +13335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A145">
         <v>2021</v>
       </c>
@@ -13364,7 +13370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A146">
         <v>2021</v>
       </c>
@@ -13399,7 +13405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A147">
         <v>2021</v>
       </c>
@@ -13434,7 +13440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A148">
         <v>2021</v>
       </c>
@@ -13469,7 +13475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A149">
         <v>2020</v>
       </c>
@@ -13504,7 +13510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A150">
         <v>2020</v>
       </c>
@@ -13609,7 +13615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A153">
         <v>2021</v>
       </c>
@@ -13679,7 +13685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A155">
         <v>2021</v>
       </c>
@@ -13714,7 +13720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A156">
         <v>2021</v>
       </c>
@@ -13749,7 +13755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A157">
         <v>2021</v>
       </c>
@@ -13784,7 +13790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A158">
         <v>2021</v>
       </c>
@@ -13819,7 +13825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A159">
         <v>2021</v>
       </c>
@@ -13854,7 +13860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A160">
         <v>2021</v>
       </c>
@@ -13889,7 +13895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A161">
         <v>2021</v>
       </c>
@@ -13924,7 +13930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A162">
         <v>2021</v>
       </c>
@@ -13959,7 +13965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A163">
         <v>2021</v>
       </c>
@@ -13994,7 +14000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A164">
         <v>2021</v>
       </c>
@@ -14029,7 +14035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A165">
         <v>2021</v>
       </c>
@@ -14064,7 +14070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A166">
         <v>2021</v>
       </c>
@@ -14099,7 +14105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A167">
         <v>2021</v>
       </c>
@@ -14134,7 +14140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A168">
         <v>2021</v>
       </c>
@@ -14169,7 +14175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A169">
         <v>2021</v>
       </c>
@@ -14204,7 +14210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A170">
         <v>2021</v>
       </c>
@@ -14239,7 +14245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A171">
         <v>2020</v>
       </c>
@@ -14274,7 +14280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A172">
         <v>2020</v>
       </c>
@@ -14309,7 +14315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A173">
         <v>2020</v>
       </c>
@@ -14344,7 +14350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A174">
         <v>2020</v>
       </c>
@@ -14379,7 +14385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A175">
         <v>2021</v>
       </c>
@@ -14414,7 +14420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A176">
         <v>2021</v>
       </c>
@@ -14449,7 +14455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A177">
         <v>2021</v>
       </c>
@@ -14484,7 +14490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A178">
         <v>2021</v>
       </c>
@@ -14519,7 +14525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A179">
         <v>2021</v>
       </c>
@@ -14554,7 +14560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A180">
         <v>2021</v>
       </c>
@@ -14589,7 +14595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A181">
         <v>2021</v>
       </c>
@@ -14624,7 +14630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A182">
         <v>2021</v>
       </c>
@@ -14659,7 +14665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A183">
         <v>2021</v>
       </c>
@@ -14694,7 +14700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A184">
         <v>2021</v>
       </c>
@@ -14729,7 +14735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A185">
         <v>2021</v>
       </c>
@@ -14764,7 +14770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A186">
         <v>2021</v>
       </c>

</xml_diff>